<commit_message>
First pass delivery form
</commit_message>
<xml_diff>
--- a/app/config/tables/colombia_registration/forms/colombia_registration/colombia_registration.xlsx
+++ b/app/config/tables/colombia_registration/forms/colombia_registration/colombia_registration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="16230" tabRatio="989" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="16230" tabRatio="989" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -343,9 +343,6 @@
     <t>colombia_registration</t>
   </si>
   <si>
-    <t>Registration</t>
-  </si>
-  <si>
     <t>rc_id</t>
   </si>
   <si>
@@ -395,6 +392,9 @@
   rcId += bPlace.slice(0, 1).toUpperCase();
   return rcId;
 })()</t>
+  </si>
+  <si>
+    <t>Registration Form</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1192,7 @@
       <c r="G13"/>
       <c r="H13"/>
       <c r="I13" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K13" s="1" t="b">
         <f>TRUE()</f>
@@ -1251,10 +1251,10 @@
         <v>13</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="K17" s="1" t="b">
         <f>TRUE()</f>
@@ -1276,11 +1276,11 @@
         <v>11</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E19" s="34"/>
       <c r="G19" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1288,10 +1288,10 @@
         <v>13</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1304,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="23.5" x14ac:dyDescent="0.55000000000000004"/>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="B5"/>
       <c r="C5" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1503,7 +1503,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -1533,7 +1533,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1666,7 +1666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1693,10 +1693,10 @@
     </row>
     <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use birthdate instead of date in the colombia forms
</commit_message>
<xml_diff>
--- a/app/config/tables/colombia_registration/forms/colombia_registration/colombia_registration.xlsx
+++ b/app/config/tables/colombia_registration/forms/colombia_registration/colombia_registration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="16230" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="16230" tabRatio="989" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="252">
   <si>
     <t>clause</t>
   </si>
@@ -819,6 +819,9 @@
   </si>
   <si>
     <t>en</t>
+  </si>
+  <si>
+    <t>birthdate</t>
   </si>
 </sst>
 </file>
@@ -1476,16 +1479,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="23.5" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.25" style="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="2" customWidth="1"/>
-    <col min="4" max="4" width="32.08203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32.125" style="3" customWidth="1"/>
     <col min="5" max="5" width="37.5" style="4" customWidth="1"/>
     <col min="6" max="8" width="35.25" style="5" customWidth="1"/>
     <col min="9" max="9" width="44" style="5" customWidth="1"/>
@@ -1493,14 +1496,14 @@
     <col min="11" max="11" width="17.25" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.75" style="1" customWidth="1"/>
     <col min="13" max="13" width="47.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="54.08203125" customWidth="1"/>
+    <col min="14" max="14" width="54.125" customWidth="1"/>
     <col min="15" max="15" width="46.25" customWidth="1"/>
-    <col min="16" max="16" width="24.6640625" customWidth="1"/>
+    <col min="16" max="16" width="24.625" customWidth="1"/>
     <col min="17" max="17" width="24.5" customWidth="1"/>
     <col min="18" max="18" width="37.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="26" customFormat="1" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" s="26" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -1556,7 +1559,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B2"/>
       <c r="C2" s="8" t="s">
         <v>11</v>
@@ -1574,7 +1577,7 @@
       <c r="J2"/>
       <c r="M2"/>
     </row>
-    <row r="3" spans="1:18" s="26" customFormat="1" ht="117.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" s="26" customFormat="1" ht="116.25" x14ac:dyDescent="0.35">
       <c r="C3" s="36" t="s">
         <v>11</v>
       </c>
@@ -1596,7 +1599,7 @@
       <c r="P3" s="27"/>
       <c r="Q3" s="27"/>
     </row>
-    <row r="4" spans="1:18" s="26" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" s="26" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>12</v>
       </c>
@@ -1607,9 +1610,9 @@
       <c r="J4" s="27"/>
       <c r="K4" s="27"/>
     </row>
-    <row r="5" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C5" s="36" t="s">
-        <v>18</v>
+        <v>251</v>
       </c>
       <c r="D5" s="37" t="s">
         <v>19</v>
@@ -1631,7 +1634,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C6" s="36" t="s">
         <v>15</v>
       </c>
@@ -1661,7 +1664,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="26" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:18" s="26" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
         <v>14</v>
       </c>
@@ -1671,7 +1674,7 @@
       <c r="I7" s="46"/>
       <c r="K7" s="27"/>
     </row>
-    <row r="8" spans="1:18" s="26" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:18" s="26" customFormat="1" ht="30.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="27" t="s">
         <v>12</v>
       </c>
@@ -1682,7 +1685,7 @@
       <c r="I8" s="46"/>
       <c r="K8" s="27"/>
     </row>
-    <row r="9" spans="1:18" s="26" customFormat="1" ht="70.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:18" s="26" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
       <c r="C9" s="36" t="s">
         <v>13</v>
       </c>
@@ -1711,7 +1714,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="26" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:18" s="26" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27" t="s">
         <v>14</v>
       </c>
@@ -1721,7 +1724,7 @@
       <c r="I10" s="46"/>
       <c r="K10" s="27"/>
     </row>
-    <row r="11" spans="1:18" s="26" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:18" s="26" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
         <v>12</v>
       </c>
@@ -1733,7 +1736,7 @@
       <c r="I11" s="47"/>
       <c r="K11" s="27"/>
     </row>
-    <row r="12" spans="1:18" s="26" customFormat="1" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:18" s="26" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B12" s="27"/>
       <c r="C12" s="36" t="s">
         <v>13</v>
@@ -1758,7 +1761,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="26" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:18" s="26" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27" t="s">
         <v>14</v>
       </c>
@@ -1770,7 +1773,7 @@
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
     </row>
-    <row r="14" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="27"/>
       <c r="C14" s="44" t="s">
         <v>11</v>
@@ -1790,7 +1793,7 @@
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
     </row>
-    <row r="15" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="27"/>
       <c r="B15" s="27"/>
       <c r="C15" s="36" t="s">
@@ -1813,7 +1816,7 @@
       <c r="L15" s="27"/>
       <c r="M15" s="27"/>
     </row>
-    <row r="16" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="27"/>
       <c r="B16" s="27"/>
       <c r="C16" s="36"/>
@@ -1828,7 +1831,7 @@
       <c r="L16" s="27"/>
       <c r="M16" s="27"/>
     </row>
-    <row r="17" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="27"/>
       <c r="B17" s="27"/>
       <c r="C17" s="36"/>
@@ -1843,7 +1846,7 @@
       <c r="L17" s="27"/>
       <c r="M17" s="27"/>
     </row>
-    <row r="18" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="27"/>
       <c r="B18" s="27"/>
       <c r="C18" s="36"/>
@@ -1858,7 +1861,7 @@
       <c r="L18" s="27"/>
       <c r="M18" s="27"/>
     </row>
-    <row r="19" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="27"/>
       <c r="B19" s="27"/>
       <c r="C19" s="36"/>
@@ -1873,7 +1876,7 @@
       <c r="L19" s="27"/>
       <c r="M19" s="27"/>
     </row>
-    <row r="20" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="27"/>
       <c r="B20" s="27"/>
       <c r="C20" s="36"/>
@@ -1888,7 +1891,7 @@
       <c r="L20" s="27"/>
       <c r="M20" s="27"/>
     </row>
-    <row r="21" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="27"/>
       <c r="B21" s="27"/>
       <c r="C21" s="36"/>
@@ -1903,7 +1906,7 @@
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
     </row>
-    <row r="22" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="27"/>
       <c r="B22" s="27"/>
       <c r="C22" s="36"/>
@@ -1918,7 +1921,7 @@
       <c r="L22" s="27"/>
       <c r="M22" s="27"/>
     </row>
-    <row r="23" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="27"/>
       <c r="B23" s="27"/>
       <c r="C23" s="36"/>
@@ -1933,7 +1936,7 @@
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
     </row>
-    <row r="24" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="27"/>
       <c r="B24" s="27"/>
       <c r="C24" s="36"/>
@@ -1948,7 +1951,7 @@
       <c r="L24" s="27"/>
       <c r="M24" s="27"/>
     </row>
-    <row r="25" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="27"/>
       <c r="B25" s="27"/>
       <c r="C25" s="36"/>
@@ -1963,7 +1966,7 @@
       <c r="L25" s="27"/>
       <c r="M25" s="27"/>
     </row>
-    <row r="26" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="27"/>
       <c r="B26" s="27"/>
       <c r="C26" s="36"/>
@@ -1978,7 +1981,7 @@
       <c r="L26" s="27"/>
       <c r="M26" s="27"/>
     </row>
-    <row r="27" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="27"/>
       <c r="B27" s="27"/>
       <c r="C27" s="36"/>
@@ -2003,18 +2006,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="23.5" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.25" style="11" customWidth="1"/>
     <col min="2" max="2" width="23" style="12" customWidth="1"/>
     <col min="3" max="3" width="8.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
@@ -2025,7 +2028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>26</v>
       </c>
@@ -2034,7 +2037,7 @@
       </c>
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>27</v>
       </c>
@@ -2043,7 +2046,7 @@
       </c>
       <c r="C3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>28</v>
       </c>
@@ -2052,7 +2055,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>29</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>245</v>
       </c>
@@ -2072,7 +2075,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>250</v>
       </c>
@@ -2094,19 +2097,19 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="23.5" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="51.25" style="3" customWidth="1"/>
     <col min="3" max="3" width="28.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" style="1" customWidth="1"/>
     <col min="5" max="9" width="8.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -2125,7 +2128,7 @@
       <c r="H1" s="16"/>
       <c r="I1" s="17"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -2142,7 +2145,7 @@
       <c r="H2" s="16"/>
       <c r="I2" s="17"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -2159,7 +2162,7 @@
       <c r="H3" s="16"/>
       <c r="I3" s="17"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -2176,7 +2179,7 @@
       <c r="H4" s="16"/>
       <c r="I4" s="17"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -2193,7 +2196,7 @@
       <c r="H5" s="16"/>
       <c r="I5" s="17"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -2210,7 +2213,7 @@
       <c r="H6" s="16"/>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -2227,7 +2230,7 @@
       <c r="H7" s="16"/>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -2244,7 +2247,7 @@
       <c r="H8" s="16"/>
       <c r="I8" s="17"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -2255,7 +2258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -2266,7 +2269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I23"/>
     </row>
   </sheetData>
@@ -2283,16 +2286,16 @@
       <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
     <col min="2" max="2" width="29.5" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.9140625" customWidth="1"/>
+    <col min="5" max="5" width="22.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>31</v>
       </c>
@@ -2309,7 +2312,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -2323,7 +2326,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2337,7 +2340,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -2379,7 +2382,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -2407,7 +2410,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -2421,7 +2424,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -2435,7 +2438,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -2449,7 +2452,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>80</v>
       </c>
@@ -2463,7 +2466,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -2491,7 +2494,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -2505,7 +2508,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -2519,7 +2522,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -2533,7 +2536,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>80</v>
       </c>
@@ -2547,7 +2550,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -2561,7 +2564,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -2575,7 +2578,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -2589,7 +2592,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -2603,7 +2606,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -2620,7 +2623,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -2637,7 +2640,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -2654,7 +2657,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -2671,7 +2674,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -2688,7 +2691,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>82</v>
       </c>
@@ -2705,7 +2708,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -2722,7 +2725,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -2739,7 +2742,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -2756,7 +2759,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2773,7 +2776,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2790,7 +2793,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -2807,7 +2810,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -2824,7 +2827,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -2841,7 +2844,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -2858,7 +2861,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>82</v>
       </c>
@@ -2875,7 +2878,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -2892,7 +2895,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -2909,7 +2912,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -2926,7 +2929,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>82</v>
       </c>
@@ -2943,7 +2946,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -2960,7 +2963,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>82</v>
       </c>
@@ -2994,7 +2997,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>82</v>
       </c>
@@ -3011,7 +3014,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>82</v>
       </c>
@@ -3028,7 +3031,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>82</v>
       </c>
@@ -3045,7 +3048,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>82</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>82</v>
       </c>
@@ -3079,7 +3082,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>82</v>
       </c>
@@ -3096,7 +3099,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>82</v>
       </c>
@@ -3113,7 +3116,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -3130,7 +3133,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>82</v>
       </c>
@@ -3147,7 +3150,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -3164,7 +3167,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -3181,7 +3184,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>82</v>
       </c>
@@ -3198,7 +3201,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>82</v>
       </c>
@@ -3215,7 +3218,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -3232,7 +3235,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>82</v>
       </c>
@@ -3249,7 +3252,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -3266,7 +3269,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -3283,7 +3286,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -3300,7 +3303,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -3317,7 +3320,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -3334,7 +3337,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>82</v>
       </c>
@@ -3351,7 +3354,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>82</v>
       </c>
@@ -3368,7 +3371,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -3385,7 +3388,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -3402,7 +3405,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>82</v>
       </c>
@@ -3419,7 +3422,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -3436,7 +3439,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -3453,7 +3456,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -3470,7 +3473,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -3487,7 +3490,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>243</v>
       </c>
@@ -3516,12 +3519,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.33203125" customWidth="1"/>
+    <col min="2" max="2" width="41.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>35</v>
       </c>
@@ -3529,7 +3532,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="170.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3537,7 +3540,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -3559,9 +3562,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>37</v>
       </c>
@@ -3578,7 +3581,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>40</v>
       </c>
@@ -3595,7 +3598,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -3626,7 +3629,7 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.25" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
@@ -3636,7 +3639,7 @@
     <col min="6" max="6" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>47</v>
       </c>
@@ -3679,13 +3682,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.375" customWidth="1"/>
     <col min="2" max="2" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>56</v>
       </c>
@@ -3693,7 +3696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>57</v>
       </c>
@@ -3701,7 +3704,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>59</v>
       </c>
@@ -3709,7 +3712,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>60</v>
       </c>
@@ -3717,7 +3720,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>61</v>
       </c>
@@ -3725,7 +3728,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>62</v>
       </c>
@@ -3733,7 +3736,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>63</v>
       </c>
@@ -3741,7 +3744,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>17</v>
       </c>
@@ -3763,14 +3766,14 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="24.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -3784,14 +3787,14 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
     </row>
-    <row r="3" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>67</v>
       </c>

</xml_diff>